<commit_message>
Done creating backend api to convert credit card pdf transaction to excel
</commit_message>
<xml_diff>
--- a/backend/output.xlsx
+++ b/backend/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,1341 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>14 Sep</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>19 Sep BUS/MRT 319783603 SINGAPORE SG Transaction Ref 74541833261288099134744</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>5.26</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>14 Sep</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>18 Sep MCDONALD'S (BDML) SINGAPORE SG Transaction Ref 74508983258015792839389</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>15 Sep</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>19 Sep BUS/MRT 320284875 SINGAPORE SG Transaction Ref 74541833261288099519464</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>5.26</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>15 Sep</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>18 Sep STUFF'D BEDOK MALL SINGAPORE SG Transaction Ref 74508983258015796112569</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>15 Sep</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>18 Sep MCDONALD'S (BDML) SINGAPORE SG Transaction Ref 74508983259015800246121</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>9.449999999999999</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>16 Sep</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>20 Sep BUS/MRT 320776484 SINGAPORE SG Transaction Ref 74541833262288082659078</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>16 Sep</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>18 Sep NTUC FP - 347 KADM SINGAPORE SG Transaction Ref 74508983259015802712666</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>6.02</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>17 Sep</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>19 Sep SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833261288072728322</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>27.49</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>17 Sep</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>19 Sep SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833261288072732258</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>27.69</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>18 Sep</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>19 Sep HUGGS GB SINGAPORE SG Transaction Ref 74103083261337564590393</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>18 Sep</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>22 Sep BUS/MRT 321745372 SINGAPORE SG Transaction Ref 74541833264288082720621</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>4.23</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>18 Sep</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>19 Sep LUCKINCOFFEE SINGAPORE SG Transaction Ref 74143253261000000853772</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>19 Sep</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>20 Sep KOPITIAM @ LAU PA S Singapore SG Bien sac lon Roti 655223 252100 aaoe az</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>19 Sep</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>21 Sep KOPI &amp; TARTS SINGAPORE SG Transaction Ref 74508983262015826380974</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>19 Sep</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>23 Sep BUS/MRT 322140993 SINGAPORE SG Transaction Ref 74541833265288082074895</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>4.23</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>19 Sep</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>20 Sep KOPITIAM @ LAU PA S Singapore SG Transaction Ref 74556223262 100949634259</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>19 Sep</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>20 Sep KOPITIAM @ LAU PA S Singapore SG Transaction Ref 74556223262100949660403</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>21 Sep</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>BUS/MRT 323041523 SINGAPORE SG Transaction Ref 74541833268288093528563</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>21 Sep</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>FAIRPRICE FINEST - SINGAPORE SG Transaction Ref 74508983264015838656377</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>26.12</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>21 Sep</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>CHATGPT SUBSCRIPTIO HTTPSOPENAI US Transaction Ref aancsccess se ne oocu</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>28.28</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>22 Sep</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>23 Sep SNP*OLD TEA HUT - O SINGAPORE SG Transaction Ref 74541833265288073482933</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>22 Sep</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>26 Sep BUS/MRT 323543852 SINGAPORE SG Transaction Ref 74541833268288097620606</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>4.23</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>22 Sep</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>23 Sep HUGGS COFFEE - CECI SINGAPORE SG Transaction Ref 74890293265102996276609</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>22 Sep</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>23 Sep KOPITIAM @ LAU PA S Singapore SG Transaction Ref 74556223265100972303829</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>8.800000000000001</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>23 Sep</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>27 Sep BUS/MRT 324021163 SINGAPORE SG Transaction Ref 74541833269288084516220</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>4.27</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>23 Sep</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>25 Sep NTUC FP - 347 KADM SINGAPORE SG Transaction Ref 74508983266015857981944</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>4.6</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>23 Sep</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>25 Sep SUPER COCONUT - 678 SINGAPORE SG Transaction Ref 74508983266015857822429</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>23 Sep</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>25 Sep FINEST PAYA LEBAR Q SINGAPORE SG Transaction Ref 74508983266015858091313</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>37.85</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>25 Sep</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>26 Sep SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833268288072540654</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>9.220000000000001</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>25 Sep</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>27 Sep ZaloraSG Singapore SG Transaction Ref 74777153268001200655072</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>106.77</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>26 Sep</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>27 Sep SEAWORLD CAFETERIA Singapore SG Transaction Ref 74556223269101001509457</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>2.3</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>26 Sep</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>30 Sep BUS/MRT 325306537 SINGAPORE SG Transaction Ref 74541833272288085254032</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>5.36</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>26 Sep</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>27 Sep KOPITIAM @ LAU PA S Singapore SG Transaction Ref 74556223269101000579147</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>26 Sep</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>28 Sep KEBABS FAKTORY SINGAPORE 0 SG Transaction Ref 74622483270698720341267</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>10.2</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>26 Sep</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>29 Sep NTUC FP - 347 KADM SINGAPORE SG Transaction Ref 74508983270015882501208</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>30.56</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>27 Sep</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>30 Sep MCDONALD'S (NP) SINGAPORE SG Transaction Ref 74508983271015890737017</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>27 Sep</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>02 Oct BUS/MRT 325758366 SINGAPORE SG Transaction Ref 74541833273288083022521</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>4.94</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>27 Sep</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>29 Sep SUBWAY - WISMA ATRI SINGAPORE SG Transaction Ref 74508983270015888233434</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>28 Sep</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>03 Oct BUS/MRT 326233999 SINGAPORE SG Transaction Ref 74541833275288098745684</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>7.54</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>28 Sep</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>30 Sep FAIRPRICE FINEST - SINGAPORE SG Transaction Ref 7450898327 1015896324869</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>28 Sep</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>30 Sep THE COFFEE BEAN - B SINGAPORE SG Transaction Ref 74541833272288077426812</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>19.9</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>29 Sep</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>02 Oct MCDONALD'S (PLSQ) SINGAPORE SG Transaction Ref 74508983273015906259939</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>29 Sep</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>03 Oct BUS/MRT 326738302 SINGAPORE SG Transaction Ref 74541833275288094529124</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>8.529999999999999</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>29 Sep</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>30 Sep KEBABCHI BRIYANI SINGAPORE SG Transaction Ref 74103803272000004200506</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>29 Sep</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>02 Oct ZaloraSG Singapore SG Transaction Ref 74777153272000201724071</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>104.5</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>29 Sep</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>10 Oct APPLE ONLINE STORE SINGAPORE 5 SG Transaction Ref 74622483282799040010024</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>29 Sep</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>07 Oct APPLE ONLINE STORE SINGAPORE 5 SG Transaction Ref 74622483279799040020051</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>30 Sep</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>02 Oct SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833273288077642797</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>44.03</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>01 Oct</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>03 Oct SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833275288072630829</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>2.35</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>01 Oct</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>03 Oct SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833275288072630811</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>01 Oct</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>03 Oct SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833275288072630795</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>02 Oct</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>03 Oct HUGGS COFFEE - CECI SINGAPORE SG Transaction Ref 74890293275102997303996</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>02 Oct</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>06 Oct BUS/MRT 328090719 SINGAPORE SG Transaction Ref 74541833278288085 101062</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>02 Oct</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>03 Oct HUGGS COFFEE - CECI SINGAPORE SG Transaction Ref 74890293275102997304960</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>02 Oct</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>03 Oct KOPITIAM @ LAU PA S Singapore SG Transaction Ref 74556223275101044024730</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>03 Oct</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>04 Oct HUGGS COFFEE - CECI SINGAPORE SG Transaction Ref 74890293276102987943107</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>03 Oct</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>07 Oct BUS/MRT 328494685 SINGAPORE SG Transaction Ref 74541833279288082131087</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>4.23</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>03 Oct</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>05 Oct KOPITIAM @ LAU PA S Singapore SG Transaction Ref 74556223277 101057163191</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>03 Oct</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>04 Oct SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833276288076328130</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>03 Oct</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>05 Oct CHUAN TAIZI MALATAN SINGAPORE 0 SG Transaction Ref 74622483277698720284593</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>14.83</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>04 Oct</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>05 Oct MADURASRESTAURANT SINGAPORE SG Transaction Ref 74143253277000001249154</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>04 Oct</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>09 Oct BUS/MRT 328962772 SINGAPORE SG Transaction Ref 74541833280288084807228</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>6.42</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>04 Oct</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>06 Oct WOK HEY - BEDOK MAL SINGAPORE SG Transaction Ref 74508983277015942646038</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>04 Oct</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>07 Oct MCDONALD'S (BDML) SINGAPORE SG Transaction Ref 745089832780159462457 11</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>05 Oct</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>07 Oct FAIRPRICE FINEST - SINGAPORE SG Transaction Ref 74508983278015950322893</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>05 Oct</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>06 Oct MOS BURGER-PAYA LEB SINGAPORE SG Transaction Ref 74541833278288076256644</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>4.65</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>05 Oct</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>10 Oct BUS/MRT 329439403 SINGAPORE SG Transaction Ref 74541833282288098005247</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>5.38</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>05 Oct</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>06 Oct KEBABCHI BRIYANI SINGAPORE SG Transaction Ref 74103803278000004 160357</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>06 Oct</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>06 Oct CDM REPAYMENT</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>06 Oct</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>07 Oct SEAWORLD CAFETERIA Singapore SG Transaction Ref 74556223279101076153544</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>06 Oct</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>07 Oct KOPITIAM @ LAU PA S Singapore SG Transaction Ref 74556223279101074474314</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>06 Oct</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>10 Oct BUS/MRT 329941783 SINGAPORE SG Transaction Ref 74541833282288097638121</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>4.24</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>06 Oct</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>07 Oct KOPITIAM @ LAU PA S Singapore SG Transaction Ref 74556223279101076334268</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>06 Oct</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>07 Oct NET*SUBWAY - ASIA S SINGAPORE SG Transaction Ref 7454183327928807 1571210</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>06 Oct</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>09 Oct GOMO MOBILE PLAN SINGAPORE SG Transaction Ref 74541833280288080299818</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>06 Oct</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>09 Oct NTUC FP - 347 KADM SINGAPORE SG Transaction Ref 74508983280015960713715</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>07 Oct</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>10 Oct SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833282288072631513</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>2.35</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>07 Oct</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>09 Oct SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833280288077704374</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>15.91</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>08 Oct</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>10 Oct SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833282288072624336</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>14.35</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>09 Oct</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>10 Oct SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833282288072626224</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>28.7</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>10 Oct</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>11 Oct 7-ELEVEN - SHENTON SINGAPORE SG Transaction Ref 74541833283288076390073</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>10 Oct</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>11 Oct KOPITIAM @ LAU PA S Singapore SG Transaction Ref 74556223283101105973908</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>10 Oct</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>11 Oct SEAWORLD CAFETERIA Singapore SG Transaction Ref 74556223283101105903814</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>10 Oct</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>14 Oct BUS/MRT 331696895 SINGAPORE SG Transaction Ref 74541833286288082481152</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>4.26</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>10 Oct</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>11 Oct SMP*MASALA EXPRESS Singapore SG Transaction Ref 24575433284310781449713</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>11 Oct</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>16 Oct BUS/MRT 332170887 SINGAPORE SG Transaction Ref 74541833287288084630805</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>6.21</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>11 Oct</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>14 Oct MCDONALD'S (BDML) SINGAPORE SG Transaction Ref 74508983285015999794574</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>12 Oct</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>14 Oct 2C2*LUCKIN COFFEE SINGAPORE SG Transaction Ref 74541833286288081254568</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>16 Oct</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>16 Oct APPLE ONLINE IPP 12 #01/12~~ Transaction Ref 74509343289001003055758</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>137.41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Created react front end to upload the pdf and convert to excel
</commit_message>
<xml_diff>
--- a/backend/output.xlsx
+++ b/backend/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,837 +441,837 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>14 Sep</t>
+          <t>15 Jul</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>19 Sep BUS/MRT 319783603 SINGAPORE SG Transaction Ref 74541833261288099134744</t>
+          <t>17 Jul 03CASHBACK</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>5.26</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>14 Sep</t>
+          <t>15 Jul</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>18 Sep MCDONALD'S (BDML) SINGAPORE SG Transaction Ref 74508983258015792839389</t>
+          <t>17 Jul SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833196288077373058</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>7.8</v>
+        <v>16.37</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>15 Sep</t>
+          <t>16 Jul</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>19 Sep BUS/MRT 320284875 SINGAPORE SG Transaction Ref 74541833261288099519464</t>
+          <t>18 Jul SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833198288072732769</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5.26</v>
+        <v>14.82</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>15 Sep</t>
+          <t>17 Jul</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>18 Sep STUFF'D BEDOK MALL SINGAPORE SG Transaction Ref 74508983258015796112569</t>
+          <t>21 Jul BUS/MRT 293403930 SINGAPORE SG Transaction Ref 74541833201288081470315</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>6.3</v>
+        <v>1.98</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>15 Sep</t>
+          <t>17 Jul</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>18 Sep MCDONALD'S (BDML) SINGAPORE SG Transaction Ref 74508983259015800246121</t>
+          <t>19 Jul THE COFFEE BEAN-ADM SINGAPORE SG TESSEGUD REL TCS REESE ZS</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>9.449999999999999</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16 Sep</t>
+          <t>17 Jul</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>20 Sep BUS/MRT 320776484 SINGAPORE SG Transaction Ref 74541833262288082659078</t>
+          <t>18 Jul RASA ISTIMEWA WATER SINGAPORE SG Transaction Ref 74143253198000001475037</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.98</v>
+        <v>9.15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>16 Sep</t>
+          <t>17 Jul</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>18 Sep NTUC FP - 347 KADM SINGAPORE SG Transaction Ref 74508983259015802712666</t>
+          <t>18 Jul www.anywheel.sg INTERNET SG Transaction Ref 24294263198000911734672</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>6.02</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>17 Sep</t>
+          <t>18 Jul</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>19 Sep SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833261288072728322</t>
+          <t>19 Jul MADURASFOOD SINGAPORE SG Transaction Ref 74143253199000000661537</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>27.49</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>17 Sep</t>
+          <t>18 Jul</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>19 Sep SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833261288072732258</t>
+          <t>19 Jul MADURASFOOD SINGAPORE SG Transaction Ref 74143253199000000884287</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>27.69</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>18 Sep</t>
+          <t>19 Jul</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>19 Sep HUGGS GB SINGAPORE SG Transaction Ref 74103083261337564590393</t>
+          <t>20 Jul GIANT UPPER PAYA LE SINGAPORE SG Transaction Ref 74541833200288074272018</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3.6</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>18 Sep</t>
+          <t>19 Jul</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>22 Sep BUS/MRT 321745372 SINGAPORE SG Transaction Ref 74541833264288082720621</t>
+          <t>20 Jul MADURASFOOD SINGAPORE SG Transaction Ref 74143253200000001161179</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>4.23</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>18 Sep</t>
+          <t>19 Jul</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>19 Sep LUCKINCOFFEE SINGAPORE SG Transaction Ref 74143253261000000853772</t>
+          <t>20 Jul MADURASFOOD SINGAPORE SG Transaction Ref 74143253200000000612800</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>4.25</v>
+        <v>14.6</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>19 Sep</t>
+          <t>19 Jul</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>20 Sep KOPITIAM @ LAU PA S Singapore SG Bien sac lon Roti 655223 252100 aaoe az</t>
+          <t>20 Jul SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833200288076229586</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>15.11</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>19 Sep</t>
+          <t>20 Jul</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>21 Sep KOPI &amp; TARTS SINGAPORE SG Transaction Ref 74508983262015826380974</t>
+          <t>21 Jul MADURASFOOD SINGAPORE SG Transaction Ref 74143253201000000635826</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>3.8</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>19 Sep</t>
+          <t>20 Jul</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>23 Sep BUS/MRT 322140993 SINGAPORE SG Transaction Ref 74541833265288082074895</t>
+          <t>21 Jul HUGGS PAYA LEBAR SINGAPORE SG Transaction Ref 74103083201328291138708</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4.23</v>
+        <v>17.3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>19 Sep</t>
+          <t>20 Jul</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>20 Sep KOPITIAM @ LAU PA S Singapore SG Transaction Ref 74556223262 100949634259</t>
+          <t>22 Jul SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833202288076545625</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>6</v>
+        <v>38.68</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>19 Sep</t>
+          <t>20 Jul</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>20 Sep KOPITIAM @ LAU PA S Singapore SG Transaction Ref 74556223262100949660403</t>
+          <t>21 Jul MADURASFOOD SINGAPORE SG Transaction Ref 74143253201000000906623</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>7.5</v>
+        <v>43.2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>21 Sep</t>
+          <t>21 Jul</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BUS/MRT 323041523 SINGAPORE SG Transaction Ref 74541833268288093528563</t>
+          <t>25 Jul BUS/MRT 295351542 SINGAPORE SG Transaction Ref 74541833205288093981156</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1.98</v>
+        <v>4.18</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>21 Sep</t>
+          <t>21 Jul</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>FAIRPRICE FINEST - SINGAPORE SG Transaction Ref 74508983264015838656377</t>
+          <t>22 Jul MADURASFOOD SINGAPORE SG Transaction Ref 74143253202000000584908</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>26.12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>21 Sep</t>
+          <t>21 Jul</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>CHATGPT SUBSCRIPTIO HTTPSOPENAI US Transaction Ref aancsccess se ne oocu</t>
+          <t>22 Jul MADURASRESTAURANT SINGAPORE SG Transaction Ref 7414325320200000097 1857</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>28.28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>22 Sep</t>
+          <t>21 Jul</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>23 Sep SNP*OLD TEA HUT - O SINGAPORE SG Transaction Ref 74541833265288073482933</t>
+          <t>21 Jul CHATGPT SUBSCRIPTIO OPENAI.COM US Transaction Ref 24492163202000015488866</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.4</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>22 Sep</t>
+          <t>22 Jul</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>26 Sep BUS/MRT 323543852 SINGAPORE SG Transaction Ref 74541833268288097620606</t>
+          <t>25 Jul NTUC FP - 347 KADM SINGAPORE SG Transaction Ref 74508983204015382145952</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>4.23</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>22 Sep</t>
+          <t>22 Jul</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>23 Sep HUGGS COFFEE - CECI SINGAPORE SG Transaction Ref 74890293265102996276609</t>
+          <t>25 Jul STARBUCKS@ADMIRALTY SINGAPORE SG Transaction Ref 7454183320528807 1571995</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>7.2</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>22 Sep</t>
+          <t>22 Jul</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>23 Sep KOPITIAM @ LAU PA S Singapore SG Transaction Ref 74556223265100972303829</t>
+          <t>25 Jul NTUC FP - 347 KADM SINGAPORE SG Transaction Ref 74508983204015382145945</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>8.800000000000001</v>
+        <v>9.130000000000001</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>23 Sep</t>
+          <t>23 Jul</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>27 Sep BUS/MRT 324021163 SINGAPORE SG Transaction Ref 74541833269288084516220</t>
+          <t>25 Jul SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833205288072669830</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>4.27</v>
+        <v>22.85</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>23 Sep</t>
+          <t>24 Jul</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>25 Sep NTUC FP - 347 KADM SINGAPORE SG Transaction Ref 74508983266015857981944</t>
+          <t>25 Jul GIANT UPPER PAYA LE SINGAPORE SG Transaction Ref 74541833205288085562899</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>4.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>23 Sep</t>
+          <t>24 Jul</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>25 Sep SUPER COCONUT - 678 SINGAPORE SG Transaction Ref 74508983266015857822429</t>
+          <t>25 Jul MADURASRESTAURANT SINGAPORE SG Transaction Ref 74143253205000000661216</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>6.3</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>23 Sep</t>
+          <t>24 Jul</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>25 Sep FINEST PAYA LEBAR Q SINGAPORE SG Transaction Ref 74508983266015858091313</t>
+          <t>25 Jul NANDHANA'S RESTAURA SINGAPORE SG Transaction Ref 74556223205212369310307</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>37.85</v>
+        <v>14.14</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>25 Sep</t>
+          <t>25 Jul</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>26 Sep SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833268288072540654</t>
+          <t>26 Jul MADURASRESTAURANT SINGAPORE SG Transaction Ref 74143253206000001 196450</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.220000000000001</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>25 Sep</t>
+          <t>25 Jul</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>27 Sep ZaloraSG Singapore SG Transaction Ref 74777153268001200655072</t>
+          <t>26 Jul MADURASRESTAURANT SINGAPORE SG Transaction Ref 741432532060000007 12588</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>106.77</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>26 Sep</t>
+          <t>25 Jul</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>27 Sep SEAWORLD CAFETERIA Singapore SG Transaction Ref 74556223269101001509457</t>
+          <t>26 Jul MADURASRESTAURANT SINGAPORE SG Transaction Ref 74143253206000001352319</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>2.3</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>26 Sep</t>
+          <t>25 Jul</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>30 Sep BUS/MRT 325306537 SINGAPORE SG Transaction Ref 74541833272288085254032</t>
+          <t>28 Jul MOS BURGER-PAYA LEB SINGAPORE SG Transaction Ref 74541833207288075937414</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>5.36</v>
+        <v>4.35</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>26 Sep</t>
+          <t>25 Jul</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>27 Sep KOPITIAM @ LAU PA S Singapore SG Transaction Ref 74556223269101000579147</t>
+          <t>26 Jul HUGGS PAYA LEBAR SINGAPORE SG Transaction Ref 74103083206329312011465</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>26 Sep</t>
+          <t>26 Jul</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>28 Sep KEBABS FAKTORY SINGAPORE 0 SG Transaction Ref 74622483270698720341267</t>
+          <t>28 Jul SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833207288076682803</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>10.2</v>
+        <v>16.07</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>26 Sep</t>
+          <t>26 Jul</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>29 Sep NTUC FP - 347 KADM SINGAPORE SG Transaction Ref 74508983270015882501208</t>
+          <t>28 Jul MR BIRYANI - CHANDE SINGAPORE SG Transaction Ref 74541833207288072386268</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>30.56</v>
+        <v>18.25</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>27 Sep</t>
+          <t>27 Jul</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>30 Sep MCDONALD'S (NP) SINGAPORE SG Transaction Ref 74508983271015890737017</t>
+          <t>31 Jul NTUC FP - 347 KADM SINGAPORE SG Transaction Ref 74508983209015419051814</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>4</v>
+        <v>5.75</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>27 Sep</t>
+          <t>27 Jul</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>02 Oct BUS/MRT 325758366 SINGAPORE SG Transaction Ref 74541833273288083022521</t>
+          <t>28 Jul OLD CHANG KEE SINGAPORE SG Transaction Ref 74556223208212264230188</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>4.94</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>27 Sep</t>
+          <t>27 Jul</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>29 Sep SUBWAY - WISMA ATRI SINGAPORE SG Transaction Ref 74508983270015888233434</t>
+          <t>31 Jul NTUC FP - 347 KADM SINGAPORE SG Transaction Ref 74508983209015419052556</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>17</v>
+        <v>12.85</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>28 Sep</t>
+          <t>05 Aug</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>03 Oct BUS/MRT 326233999 SINGAPORE SG Transaction Ref 74541833275288098745684</t>
+          <t>07 Aug MOHD MUSTAFA SAMS SINGAPORE SG Transaction Ref 74103083217330367778567</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>7.54</v>
+        <v>39.3</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>28 Sep</t>
+          <t>06 Aug</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>30 Sep FAIRPRICE FINEST - SINGAPORE SG Transaction Ref 7450898327 1015896324869</t>
+          <t>08 Aug THE COFFEE BEAN-ADM SINGAPORE SG Transaction Ref 74541833219288073888482</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>12.7</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>28 Sep</t>
+          <t>06 Aug</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>30 Sep THE COFFEE BEAN - B SINGAPORE SG Transaction Ref 74541833272288077426812</t>
+          <t>08 Aug NTUC FP - 347 KADM SINGAPORE SG Transaction Ref 74508983218015492935338</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>19.9</v>
+        <v>8.15</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>29 Sep</t>
+          <t>06 Aug</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>02 Oct MCDONALD'S (PLSQ) SINGAPORE SG Transaction Ref 74508983273015906259939</t>
+          <t>08 Aug MOS BURGER-KPG ADMI SINGAPORE SG Transaction Ref 7454183321928807 1360856</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>7.75</v>
+        <v>8.550000000000001</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>29 Sep</t>
+          <t>06 Aug</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>03 Oct BUS/MRT 326738302 SINGAPORE SG Transaction Ref 74541833275288094529124</t>
+          <t>08 Aug SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833219288072852984</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>8.529999999999999</v>
+        <v>9.93</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>29 Sep</t>
+          <t>06 Aug</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>30 Sep KEBABCHI BRIYANI SINGAPORE SG Transaction Ref 74103803272000004200506</t>
+          <t>07 Aug A MEDIUM CORPORATIO 4155085008 US Transaction Ref aes sss se so0D</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>17</v>
+        <v>69.55</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>29 Sep</t>
+          <t>07 Aug</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>02 Oct ZaloraSG Singapore SG Transaction Ref 74777153272000201724071</t>
+          <t>08 Aug SEAWORLD CAFETERIA Singapore SG Transaction Ref 74556223219100632688491</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>104.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>29 Sep</t>
+          <t>07 Aug</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>10 Oct APPLE ONLINE STORE SINGAPORE 5 SG Transaction Ref 74622483282799040010024</t>
+          <t>08 Aug HUGGS GB SINGAPORE SG Transaction Ref 74103083219331376835677</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>350</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>29 Sep</t>
+          <t>07 Aug</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>07 Oct APPLE ONLINE STORE SINGAPORE 5 SG Transaction Ref 74622483279799040020051</t>
+          <t>08 Aug TANAMERA PTE LTD SINGAPORE SG Transaction Ref 74541833219288081413695</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1299</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>30 Sep</t>
+          <t>07 Aug</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>02 Oct SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833273288077642797</t>
+          <t>08 Aug www.anywheel.sg INTERNET SG Transaction Ref 24294263219001303611317</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>44.03</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>01 Oct</t>
+          <t>07 Aug</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>03 Oct SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833275288072630829</t>
+          <t>08 Aug NANDHANA'S RESTAURA Singapore SG Transaction Ref 74556223219100631766314</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>2.35</v>
+        <v>15.21</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>01 Oct</t>
+          <t>09 Aug</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>03 Oct SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833275288072630811</t>
+          <t>12 Aug NTUC FP - 347 KADM SINGAPORE SG Transaction Ref 74508883222016520396614</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2.85</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>01 Oct</t>
+          <t>09 Aug</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>03 Oct SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833275288072630795</t>
+          <t>12 Aug MCDONALD'S (AMT2) SINGAPORE SG Transaction Ref 74508983222015520993311</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>13.8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>02 Oct</t>
+          <t>09 Aug</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>03 Oct HUGGS COFFEE - CECI SINGAPORE SG Transaction Ref 74890293275102997303996</t>
+          <t>11 Aug SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833222288072660168</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>3.6</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>02 Oct</t>
+          <t>09 Aug</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>06 Oct BUS/MRT 328090719 SINGAPORE SG Transaction Ref 74541833278288085 101062</t>
+          <t>11 Aug NTUC FP - 347 KADM SINGAPORE SG Transaction Ref 74508983221015515513109</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>4.25</v>
+        <v>12.48</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>02 Oct</t>
+          <t>09 Aug</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>03 Oct HUGGS COFFEE - CECI SINGAPORE SG Transaction Ref 74890293275102997304960</t>
+          <t>12 Aug NTUC FP - 347 KADM SINGAPORE SG Transaction Ref 74508983222015520396606</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>5.5</v>
+        <v>13.82</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>02 Oct</t>
+          <t>10 Aug</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>03 Oct KOPITIAM @ LAU PA S Singapore SG Transaction Ref 74556223275101044024730</t>
+          <t>11 Aug COPPER CHIMNEY EXPR SINGAPORE SG Transaction Ref 74103083222331391 184494</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>6</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>03 Oct</t>
+          <t>10 Aug</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>04 Oct HUGGS COFFEE - CECI SINGAPORE SG Transaction Ref 74890293276102987943107</t>
+          <t>11 Aug HUGGS GB SINGAPORE SG Transaction Ref 74103083222331391 155981</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1281,496 +1281,301 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>03 Oct</t>
+          <t>10 Aug</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>07 Oct BUS/MRT 328494685 SINGAPORE SG Transaction Ref 74541833279288082131087</t>
+          <t>11 Aug ANGLO INDIAN CAFE &amp; SINGAPORE SG Transaction Ref 74541833222288081343632</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>4.23</v>
+        <v>6.48</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>03 Oct</t>
+          <t>10 Aug</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>05 Oct KOPITIAM @ LAU PA S Singapore SG Transaction Ref 74556223277 101057163191</t>
+          <t>11 Aug COPPER CHIMNEY EXPR SINGAPORE SG Transaction Ref 74103083222331391 184379</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>03 Oct</t>
+          <t>10 Aug</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>04 Oct SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833276288076328130</t>
+          <t>12 Aug BISMILLAH BIRYANI - SINGAPORE SG Transaction Ref 74508983222015523429347</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>13</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>03 Oct</t>
+          <t>11 Aug</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>05 Oct CHUAN TAIZI MALATAN SINGAPORE 0 SG Transaction Ref 74622483277698720284593</t>
+          <t>12 Aug SEAWORLD CAFETERIA Singapore SG Transaction Ref 74556223223100664034857</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>14.83</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>04 Oct</t>
+          <t>11 Aug</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>05 Oct MADURASRESTAURANT SINGAPORE SG Transaction Ref 74143253277000001249154</t>
+          <t>12 Aug SEAWORLD CAFETERIA Singapore SG Transaction Ref 74556223223100664026028</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1.4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>04 Oct</t>
+          <t>11 Aug</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>09 Oct BUS/MRT 328962772 SINGAPORE SG Transaction Ref 74541833280288084807228</t>
+          <t>12 Aug SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833223288076527818</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>6.42</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>04 Oct</t>
+          <t>11 Aug</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>06 Oct WOK HEY - BEDOK MAL SINGAPORE SG Transaction Ref 74508983277015942646038</t>
+          <t>12 Aug GOODDAY FOOD PTE LT SINGAPORE SG Transaction Ref 74103083223331395490698</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>6.9</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>04 Oct</t>
+          <t>12 Aug</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>07 Oct MCDONALD'S (BDML) SINGAPORE SG Transaction Ref 745089832780159462457 11</t>
+          <t>16 Aug BUS/MRT 304986709 SINGAPORE SG Transaction Ref 74541833227288084224750</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>8.5</v>
+        <v>3.09</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>05 Oct</t>
+          <t>12 Aug</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>07 Oct FAIRPRICE FINEST - SINGAPORE SG Transaction Ref 74508983278015950322893</t>
+          <t>14 Aug NANDHANA'S RESTAURA Singapore SG Transaction Ref 74556223224 100668751380</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>3.02</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>05 Oct</t>
+          <t>12 Aug</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>06 Oct MOS BURGER-PAYA LEB SINGAPORE SG Transaction Ref 74541833278288076256644</t>
+          <t>14 Aug SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833224288077587968</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>4.65</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>05 Oct</t>
+          <t>13 Aug</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>10 Oct BUS/MRT 329439403 SINGAPORE SG Transaction Ref 74541833282288098005247</t>
+          <t>16 Aug MCDONALD'S (AMT2) SINGAPORE SG Transaction Ref 74508983226015552029477</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>5.38</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>05 Oct</t>
+          <t>13 Aug</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>06 Oct KEBABCHI BRIYANI SINGAPORE SG Transaction Ref 74103803278000004 160357</t>
+          <t>15 Aug SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 745418332262880727 14508</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>19.5</v>
+        <v>13.13</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>06 Oct</t>
+          <t>14 Aug</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>06 Oct CDM REPAYMENT</t>
+          <t>15 Aug GIANT UPPER PAYA LE SINGAPORE SG Transaction Ref 74541833226288085380560</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>800</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>06 Oct</t>
+          <t>14 Aug</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>07 Oct SEAWORLD CAFETERIA Singapore SG Transaction Ref 74556223279101076153544</t>
+          <t>16 Aug THE COFFEE BEAN - B SINGAPORE SG Transaction Ref 74541833227288076980807</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>3.4</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>06 Oct</t>
+          <t>14 Aug</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>07 Oct KOPITIAM @ LAU PA S Singapore SG Transaction Ref 74556223279101074474314</t>
+          <t>15 Aug MADURASRESTAURANT SINGAPORE SG Transaction Ref 74143253226000001299854</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>3.5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>06 Oct</t>
+          <t>15 Aug</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>10 Oct BUS/MRT 329941783 SINGAPORE SG Transaction Ref 74541833282288097638121</t>
+          <t>16 Aug SNP*OLD TEA HUT - O SINGAPORE SG Transaction Ref 74541833227288073177878</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>4.24</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>06 Oct</t>
+          <t>15 Aug</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>07 Oct KOPITIAM @ LAU PA S Singapore SG Transaction Ref 74556223279101076334268</t>
+          <t>16 Aug SNP*PASTA E FORMAGG SINGAPORE SG Transaction Ref 74541833227288073186424</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7.5</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>06 Oct</t>
+          <t>15 Aug</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>07 Oct NET*SUBWAY - ASIA S SINGAPORE SG Transaction Ref 7454183327928807 1571210</t>
+          <t>16 Aug GOODDAY FOOD PTE LT SINGAPORE SG Transaction Ref 74103083227332412587835</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>10</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>06 Oct</t>
+          <t>15 Aug</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>09 Oct GOMO MOBILE PLAN SINGAPORE SG Transaction Ref 74541833280288080299818</t>
+          <t>16 Aug COPPER CHIMNEY EXPR SINGAPORE SG Transaction Ref 74103083227332412543861</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>12</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>06 Oct</t>
+          <t>15 Aug</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>09 Oct NTUC FP - 347 KADM SINGAPORE SG Transaction Ref 74508983280015960713715</t>
+          <t>16 Aug SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833227288076423014</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>19.8</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>07 Oct</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>10 Oct SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833282288072631513</t>
-        </is>
-      </c>
-      <c r="C78" t="n">
-        <v>2.35</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>07 Oct</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>09 Oct SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833280288077704374</t>
-        </is>
-      </c>
-      <c r="C79" t="n">
-        <v>15.91</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>08 Oct</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>10 Oct SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833282288072624336</t>
-        </is>
-      </c>
-      <c r="C80" t="n">
-        <v>14.35</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>09 Oct</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>10 Oct SHENGSIONG@785EWOOD SINGAPORE SG Transaction Ref 74541833282288072626224</t>
-        </is>
-      </c>
-      <c r="C81" t="n">
-        <v>28.7</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>10 Oct</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>11 Oct 7-ELEVEN - SHENTON SINGAPORE SG Transaction Ref 74541833283288076390073</t>
-        </is>
-      </c>
-      <c r="C82" t="n">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>10 Oct</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>11 Oct KOPITIAM @ LAU PA S Singapore SG Transaction Ref 74556223283101105973908</t>
-        </is>
-      </c>
-      <c r="C83" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>10 Oct</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>11 Oct SEAWORLD CAFETERIA Singapore SG Transaction Ref 74556223283101105903814</t>
-        </is>
-      </c>
-      <c r="C84" t="n">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>10 Oct</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>14 Oct BUS/MRT 331696895 SINGAPORE SG Transaction Ref 74541833286288082481152</t>
-        </is>
-      </c>
-      <c r="C85" t="n">
-        <v>4.26</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>10 Oct</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>11 Oct SMP*MASALA EXPRESS Singapore SG Transaction Ref 24575433284310781449713</t>
-        </is>
-      </c>
-      <c r="C86" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>11 Oct</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>16 Oct BUS/MRT 332170887 SINGAPORE SG Transaction Ref 74541833287288084630805</t>
-        </is>
-      </c>
-      <c r="C87" t="n">
-        <v>6.21</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>11 Oct</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>14 Oct MCDONALD'S (BDML) SINGAPORE SG Transaction Ref 74508983285015999794574</t>
-        </is>
-      </c>
-      <c r="C88" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>12 Oct</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>14 Oct 2C2*LUCKIN COFFEE SINGAPORE SG Transaction Ref 74541833286288081254568</t>
-        </is>
-      </c>
-      <c r="C89" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>16 Oct</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>16 Oct APPLE ONLINE IPP 12 #01/12~~ Transaction Ref 74509343289001003055758</t>
-        </is>
-      </c>
-      <c r="C90" t="n">
-        <v>137.41</v>
+        <v>16.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>